<commit_message>
Update ccar-cic Codice di Diritto Canonico. Internal link x ObsidianMD a Canoni e Commi.xlsx
</commit_message>
<xml_diff>
--- a/Chiesa/Documenti vari/ccar-cic Codice di Diritto Canonico. Internal link x ObsidianMD a Canoni e Commi.xlsx
+++ b/Chiesa/Documenti vari/ccar-cic Codice di Diritto Canonico. Internal link x ObsidianMD a Canoni e Commi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\EmanueleTinari\Obsidian\Chiesa\Documenti vari\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{263C4E58-A999-4FD2-994C-8A833EC7CE73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F83795D-B971-4FFE-B7CF-A5DA009C72B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{7E4545D9-FEFC-4991-8583-F42C0BB78B5F}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9242" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9191" uniqueCount="10">
   <si>
     <t>-c2|Cm 2]]</t>
   </si>
@@ -513,8 +513,8 @@
   <sheetPr codeName="Foglio1"/>
   <dimension ref="A1:S1753"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A319" workbookViewId="0">
-      <selection activeCell="A330" sqref="A330"/>
+    <sheetView tabSelected="1" topLeftCell="A349" workbookViewId="0">
+      <selection activeCell="A368" sqref="A368"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.58203125" defaultRowHeight="13"/>
@@ -9349,14 +9349,14 @@
         <v>1</v>
       </c>
       <c r="H266" s="1" t="str">
-        <f t="shared" ref="H265:H328" si="16">_xlfn.CONCAT(F266,B266,G266)</f>
+        <f t="shared" ref="H266:H326" si="16">_xlfn.CONCAT(F266,B266,G266)</f>
         <v>[[Documenti vari/ccar-cic#^ccar-cic-c266-c1|Cm 1]]</v>
       </c>
       <c r="I266" s="2" t="s">
         <v>0</v>
       </c>
       <c r="J266" s="1" t="str">
-        <f t="shared" ref="J265:J328" si="17">_xlfn.CONCAT(F266,B266,I266)</f>
+        <f t="shared" ref="J266:J326" si="17">_xlfn.CONCAT(F266,B266,I266)</f>
         <v>[[Documenti vari/ccar-cic#^ccar-cic-c266-c2|Cm 2]]</v>
       </c>
       <c r="K266" s="1" t="s">
@@ -11546,1489 +11546,1329 @@
         <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 329|Canone 329]] -  -  -  -  -  - </v>
       </c>
     </row>
-    <row r="330" spans="1:19" ht="13.5" thickTop="1">
-      <c r="A330" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B330" s="9">
+    <row r="330" spans="1:19" s="1" customFormat="1" ht="14" thickTop="1" thickBot="1">
+      <c r="A330" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B330" s="3">
         <v>330</v>
       </c>
-      <c r="C330" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D330" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E330" s="9" t="str">
+      <c r="C330" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D330" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E330" s="3" t="str">
         <f t="shared" si="18"/>
         <v>[[Documenti vari/ccar-cic#Canone 330|Canone 330]]</v>
       </c>
-      <c r="F330" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="G330" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="H330" s="9" t="str">
-        <f t="shared" ref="H329:H392" si="20">_xlfn.CONCAT(F330,B330,G330)</f>
-        <v>[[Documenti vari/ccar-cic#^ccar-cic-c330-c1|Cm 1]]</v>
-      </c>
-      <c r="I330" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="J330" s="9" t="str">
-        <f t="shared" ref="J329:J392" si="21">_xlfn.CONCAT(F330,B330,I330)</f>
-        <v>[[Documenti vari/ccar-cic#^ccar-cic-c330-c2|Cm 2]]</v>
-      </c>
-      <c r="S330" s="9" t="str">
+      <c r="F330" s="3"/>
+      <c r="G330" s="4"/>
+      <c r="H330" s="3"/>
+      <c r="I330" s="4"/>
+      <c r="J330" s="3"/>
+      <c r="K330" s="3"/>
+      <c r="L330" s="3"/>
+      <c r="M330" s="3"/>
+      <c r="N330" s="3"/>
+      <c r="O330" s="3"/>
+      <c r="P330" s="3"/>
+      <c r="Q330" s="3"/>
+      <c r="R330" s="3"/>
+      <c r="S330" s="3" t="str">
         <f t="shared" si="19"/>
-        <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 330|Canone 330]] - [[Documenti vari/ccar-cic#^ccar-cic-c330-c1|Cm 1]] - [[Documenti vari/ccar-cic#^ccar-cic-c330-c2|Cm 2]] -  -  -  - </v>
-      </c>
-    </row>
-    <row r="331" spans="1:19">
-      <c r="A331" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B331" s="9">
+        <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 330|Canone 330]] -  -  -  -  -  - </v>
+      </c>
+    </row>
+    <row r="331" spans="1:19" s="1" customFormat="1" ht="13.5" thickTop="1">
+      <c r="A331" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B331" s="1">
         <v>331</v>
       </c>
-      <c r="C331" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D331" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E331" s="9" t="str">
+      <c r="C331" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D331" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E331" s="1" t="str">
         <f t="shared" si="18"/>
         <v>[[Documenti vari/ccar-cic#Canone 331|Canone 331]]</v>
       </c>
-      <c r="F331" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="G331" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="H331" s="9" t="str">
-        <f t="shared" si="20"/>
-        <v>[[Documenti vari/ccar-cic#^ccar-cic-c331-c1|Cm 1]]</v>
-      </c>
-      <c r="I331" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="J331" s="9" t="str">
-        <f t="shared" si="21"/>
-        <v>[[Documenti vari/ccar-cic#^ccar-cic-c331-c2|Cm 2]]</v>
-      </c>
-      <c r="S331" s="9" t="str">
+      <c r="G331" s="2"/>
+      <c r="I331" s="2"/>
+      <c r="S331" s="1" t="str">
         <f t="shared" si="19"/>
-        <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 331|Canone 331]] - [[Documenti vari/ccar-cic#^ccar-cic-c331-c1|Cm 1]] - [[Documenti vari/ccar-cic#^ccar-cic-c331-c2|Cm 2]] -  -  -  - </v>
-      </c>
-    </row>
-    <row r="332" spans="1:19">
-      <c r="A332" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B332" s="9">
+        <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 331|Canone 331]] -  -  -  -  -  - </v>
+      </c>
+    </row>
+    <row r="332" spans="1:19" s="1" customFormat="1">
+      <c r="A332" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B332" s="1">
         <v>332</v>
       </c>
-      <c r="C332" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D332" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E332" s="9" t="str">
+      <c r="C332" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D332" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E332" s="1" t="str">
         <f t="shared" si="18"/>
         <v>[[Documenti vari/ccar-cic#Canone 332|Canone 332]]</v>
       </c>
-      <c r="F332" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="G332" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="H332" s="9" t="str">
-        <f t="shared" si="20"/>
+      <c r="F332" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G332" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H332" s="1" t="str">
+        <f t="shared" ref="H330:H392" si="20">_xlfn.CONCAT(F332,B332,G332)</f>
         <v>[[Documenti vari/ccar-cic#^ccar-cic-c332-c1|Cm 1]]</v>
       </c>
-      <c r="I332" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="J332" s="9" t="str">
-        <f t="shared" si="21"/>
+      <c r="I332" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J332" s="1" t="str">
+        <f t="shared" ref="J330:J392" si="21">_xlfn.CONCAT(F332,B332,I332)</f>
         <v>[[Documenti vari/ccar-cic#^ccar-cic-c332-c2|Cm 2]]</v>
       </c>
-      <c r="S332" s="9" t="str">
+      <c r="S332" s="1" t="str">
         <f t="shared" si="19"/>
         <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 332|Canone 332]] - [[Documenti vari/ccar-cic#^ccar-cic-c332-c1|Cm 1]] - [[Documenti vari/ccar-cic#^ccar-cic-c332-c2|Cm 2]] -  -  -  - </v>
       </c>
     </row>
-    <row r="333" spans="1:19">
-      <c r="A333" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B333" s="9">
+    <row r="333" spans="1:19" s="1" customFormat="1">
+      <c r="A333" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B333" s="1">
         <v>333</v>
       </c>
-      <c r="C333" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D333" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E333" s="9" t="str">
+      <c r="C333" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D333" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E333" s="1" t="str">
         <f t="shared" si="18"/>
         <v>[[Documenti vari/ccar-cic#Canone 333|Canone 333]]</v>
       </c>
-      <c r="F333" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="G333" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="H333" s="9" t="str">
+      <c r="F333" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G333" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H333" s="1" t="str">
         <f t="shared" si="20"/>
         <v>[[Documenti vari/ccar-cic#^ccar-cic-c333-c1|Cm 1]]</v>
       </c>
-      <c r="I333" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="J333" s="9" t="str">
+      <c r="I333" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J333" s="1" t="str">
         <f t="shared" si="21"/>
         <v>[[Documenti vari/ccar-cic#^ccar-cic-c333-c2|Cm 2]]</v>
       </c>
-      <c r="S333" s="9" t="str">
+      <c r="K333" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L333" s="1" t="str">
+        <f>_xlfn.CONCAT(F333,B333,K333)</f>
+        <v>[[Documenti vari/ccar-cic#^ccar-cic-c333-c3|Cm 3]]</v>
+      </c>
+      <c r="S333" s="1" t="str">
         <f t="shared" si="19"/>
-        <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 333|Canone 333]] - [[Documenti vari/ccar-cic#^ccar-cic-c333-c1|Cm 1]] - [[Documenti vari/ccar-cic#^ccar-cic-c333-c2|Cm 2]] -  -  -  - </v>
-      </c>
-    </row>
-    <row r="334" spans="1:19">
-      <c r="A334" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B334" s="9">
+        <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 333|Canone 333]] - [[Documenti vari/ccar-cic#^ccar-cic-c333-c1|Cm 1]] - [[Documenti vari/ccar-cic#^ccar-cic-c333-c2|Cm 2]] - [[Documenti vari/ccar-cic#^ccar-cic-c333-c3|Cm 3]] -  -  - </v>
+      </c>
+    </row>
+    <row r="334" spans="1:19" s="1" customFormat="1">
+      <c r="A334" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B334" s="1">
         <v>334</v>
       </c>
-      <c r="C334" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D334" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E334" s="9" t="str">
+      <c r="C334" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D334" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E334" s="1" t="str">
         <f t="shared" si="18"/>
         <v>[[Documenti vari/ccar-cic#Canone 334|Canone 334]]</v>
       </c>
-      <c r="F334" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="G334" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="H334" s="9" t="str">
-        <f t="shared" si="20"/>
-        <v>[[Documenti vari/ccar-cic#^ccar-cic-c334-c1|Cm 1]]</v>
-      </c>
-      <c r="I334" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="J334" s="9" t="str">
-        <f t="shared" si="21"/>
-        <v>[[Documenti vari/ccar-cic#^ccar-cic-c334-c2|Cm 2]]</v>
-      </c>
-      <c r="S334" s="9" t="str">
+      <c r="G334" s="2"/>
+      <c r="I334" s="2"/>
+      <c r="S334" s="1" t="str">
         <f t="shared" si="19"/>
-        <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 334|Canone 334]] - [[Documenti vari/ccar-cic#^ccar-cic-c334-c1|Cm 1]] - [[Documenti vari/ccar-cic#^ccar-cic-c334-c2|Cm 2]] -  -  -  - </v>
-      </c>
-    </row>
-    <row r="335" spans="1:19">
-      <c r="A335" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B335" s="9">
+        <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 334|Canone 334]] -  -  -  -  -  - </v>
+      </c>
+    </row>
+    <row r="335" spans="1:19" s="1" customFormat="1" ht="13.5" thickBot="1">
+      <c r="A335" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B335" s="3">
         <v>335</v>
       </c>
-      <c r="C335" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D335" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E335" s="9" t="str">
+      <c r="C335" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D335" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E335" s="3" t="str">
         <f t="shared" si="18"/>
         <v>[[Documenti vari/ccar-cic#Canone 335|Canone 335]]</v>
       </c>
-      <c r="F335" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="G335" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="H335" s="9" t="str">
-        <f t="shared" si="20"/>
-        <v>[[Documenti vari/ccar-cic#^ccar-cic-c335-c1|Cm 1]]</v>
-      </c>
-      <c r="I335" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="J335" s="9" t="str">
-        <f t="shared" si="21"/>
-        <v>[[Documenti vari/ccar-cic#^ccar-cic-c335-c2|Cm 2]]</v>
-      </c>
-      <c r="S335" s="9" t="str">
+      <c r="F335" s="3"/>
+      <c r="G335" s="4"/>
+      <c r="H335" s="3"/>
+      <c r="I335" s="4"/>
+      <c r="J335" s="3"/>
+      <c r="K335" s="3"/>
+      <c r="L335" s="3"/>
+      <c r="M335" s="3"/>
+      <c r="N335" s="3"/>
+      <c r="O335" s="3"/>
+      <c r="P335" s="3"/>
+      <c r="Q335" s="3"/>
+      <c r="R335" s="3"/>
+      <c r="S335" s="3" t="str">
         <f t="shared" si="19"/>
-        <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 335|Canone 335]] - [[Documenti vari/ccar-cic#^ccar-cic-c335-c1|Cm 1]] - [[Documenti vari/ccar-cic#^ccar-cic-c335-c2|Cm 2]] -  -  -  - </v>
-      </c>
-    </row>
-    <row r="336" spans="1:19">
-      <c r="A336" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B336" s="9">
+        <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 335|Canone 335]] -  -  -  -  -  - </v>
+      </c>
+    </row>
+    <row r="336" spans="1:19" s="1" customFormat="1" ht="13.5" thickTop="1">
+      <c r="A336" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B336" s="1">
         <v>336</v>
       </c>
-      <c r="C336" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D336" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E336" s="9" t="str">
+      <c r="C336" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D336" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E336" s="1" t="str">
         <f t="shared" si="18"/>
         <v>[[Documenti vari/ccar-cic#Canone 336|Canone 336]]</v>
       </c>
-      <c r="F336" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="G336" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="H336" s="9" t="str">
-        <f t="shared" si="20"/>
-        <v>[[Documenti vari/ccar-cic#^ccar-cic-c336-c1|Cm 1]]</v>
-      </c>
-      <c r="I336" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="J336" s="9" t="str">
-        <f t="shared" si="21"/>
-        <v>[[Documenti vari/ccar-cic#^ccar-cic-c336-c2|Cm 2]]</v>
-      </c>
-      <c r="S336" s="9" t="str">
+      <c r="G336" s="2"/>
+      <c r="I336" s="2"/>
+      <c r="S336" s="1" t="str">
         <f t="shared" si="19"/>
-        <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 336|Canone 336]] - [[Documenti vari/ccar-cic#^ccar-cic-c336-c1|Cm 1]] - [[Documenti vari/ccar-cic#^ccar-cic-c336-c2|Cm 2]] -  -  -  - </v>
-      </c>
-    </row>
-    <row r="337" spans="1:19">
-      <c r="A337" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B337" s="9">
+        <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 336|Canone 336]] -  -  -  -  -  - </v>
+      </c>
+    </row>
+    <row r="337" spans="1:19" s="1" customFormat="1">
+      <c r="A337" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B337" s="1">
         <v>337</v>
       </c>
-      <c r="C337" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D337" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E337" s="9" t="str">
+      <c r="C337" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D337" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E337" s="1" t="str">
         <f t="shared" si="18"/>
         <v>[[Documenti vari/ccar-cic#Canone 337|Canone 337]]</v>
       </c>
-      <c r="F337" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="G337" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="H337" s="9" t="str">
+      <c r="F337" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G337" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H337" s="1" t="str">
         <f t="shared" si="20"/>
         <v>[[Documenti vari/ccar-cic#^ccar-cic-c337-c1|Cm 1]]</v>
       </c>
-      <c r="I337" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="J337" s="9" t="str">
+      <c r="I337" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J337" s="1" t="str">
         <f t="shared" si="21"/>
         <v>[[Documenti vari/ccar-cic#^ccar-cic-c337-c2|Cm 2]]</v>
       </c>
-      <c r="S337" s="9" t="str">
+      <c r="K337" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L337" s="1" t="str">
+        <f>_xlfn.CONCAT(F337,B337,K337)</f>
+        <v>[[Documenti vari/ccar-cic#^ccar-cic-c337-c3|Cm 3]]</v>
+      </c>
+      <c r="S337" s="1" t="str">
         <f t="shared" si="19"/>
-        <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 337|Canone 337]] - [[Documenti vari/ccar-cic#^ccar-cic-c337-c1|Cm 1]] - [[Documenti vari/ccar-cic#^ccar-cic-c337-c2|Cm 2]] -  -  -  - </v>
-      </c>
-    </row>
-    <row r="338" spans="1:19">
-      <c r="A338" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B338" s="9">
+        <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 337|Canone 337]] - [[Documenti vari/ccar-cic#^ccar-cic-c337-c1|Cm 1]] - [[Documenti vari/ccar-cic#^ccar-cic-c337-c2|Cm 2]] - [[Documenti vari/ccar-cic#^ccar-cic-c337-c3|Cm 3]] -  -  - </v>
+      </c>
+    </row>
+    <row r="338" spans="1:19" s="1" customFormat="1">
+      <c r="A338" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B338" s="1">
         <v>338</v>
       </c>
-      <c r="C338" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D338" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E338" s="9" t="str">
+      <c r="C338" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D338" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E338" s="1" t="str">
         <f t="shared" si="18"/>
         <v>[[Documenti vari/ccar-cic#Canone 338|Canone 338]]</v>
       </c>
-      <c r="F338" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="G338" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="H338" s="9" t="str">
+      <c r="F338" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G338" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H338" s="1" t="str">
         <f t="shared" si="20"/>
         <v>[[Documenti vari/ccar-cic#^ccar-cic-c338-c1|Cm 1]]</v>
       </c>
-      <c r="I338" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="J338" s="9" t="str">
+      <c r="I338" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J338" s="1" t="str">
         <f t="shared" si="21"/>
         <v>[[Documenti vari/ccar-cic#^ccar-cic-c338-c2|Cm 2]]</v>
       </c>
-      <c r="S338" s="9" t="str">
+      <c r="S338" s="1" t="str">
         <f t="shared" si="19"/>
         <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 338|Canone 338]] - [[Documenti vari/ccar-cic#^ccar-cic-c338-c1|Cm 1]] - [[Documenti vari/ccar-cic#^ccar-cic-c338-c2|Cm 2]] -  -  -  - </v>
       </c>
     </row>
-    <row r="339" spans="1:19">
-      <c r="A339" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B339" s="9">
+    <row r="339" spans="1:19" s="1" customFormat="1">
+      <c r="A339" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B339" s="1">
         <v>339</v>
       </c>
-      <c r="C339" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D339" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E339" s="9" t="str">
+      <c r="C339" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D339" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E339" s="1" t="str">
         <f t="shared" si="18"/>
         <v>[[Documenti vari/ccar-cic#Canone 339|Canone 339]]</v>
       </c>
-      <c r="F339" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="G339" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="H339" s="9" t="str">
+      <c r="F339" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G339" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H339" s="1" t="str">
         <f t="shared" si="20"/>
         <v>[[Documenti vari/ccar-cic#^ccar-cic-c339-c1|Cm 1]]</v>
       </c>
-      <c r="I339" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="J339" s="9" t="str">
+      <c r="I339" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J339" s="1" t="str">
         <f t="shared" si="21"/>
         <v>[[Documenti vari/ccar-cic#^ccar-cic-c339-c2|Cm 2]]</v>
       </c>
-      <c r="S339" s="9" t="str">
+      <c r="S339" s="1" t="str">
         <f t="shared" si="19"/>
         <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 339|Canone 339]] - [[Documenti vari/ccar-cic#^ccar-cic-c339-c1|Cm 1]] - [[Documenti vari/ccar-cic#^ccar-cic-c339-c2|Cm 2]] -  -  -  - </v>
       </c>
     </row>
-    <row r="340" spans="1:19">
-      <c r="A340" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B340" s="9">
+    <row r="340" spans="1:19" s="1" customFormat="1">
+      <c r="A340" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B340" s="1">
         <v>340</v>
       </c>
-      <c r="C340" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D340" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E340" s="9" t="str">
+      <c r="C340" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D340" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E340" s="1" t="str">
         <f t="shared" si="18"/>
         <v>[[Documenti vari/ccar-cic#Canone 340|Canone 340]]</v>
       </c>
-      <c r="F340" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="G340" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="H340" s="9" t="str">
-        <f t="shared" si="20"/>
-        <v>[[Documenti vari/ccar-cic#^ccar-cic-c340-c1|Cm 1]]</v>
-      </c>
-      <c r="I340" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="J340" s="9" t="str">
-        <f t="shared" si="21"/>
-        <v>[[Documenti vari/ccar-cic#^ccar-cic-c340-c2|Cm 2]]</v>
-      </c>
-      <c r="S340" s="9" t="str">
+      <c r="G340" s="2"/>
+      <c r="I340" s="2"/>
+      <c r="S340" s="1" t="str">
         <f t="shared" si="19"/>
-        <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 340|Canone 340]] - [[Documenti vari/ccar-cic#^ccar-cic-c340-c1|Cm 1]] - [[Documenti vari/ccar-cic#^ccar-cic-c340-c2|Cm 2]] -  -  -  - </v>
-      </c>
-    </row>
-    <row r="341" spans="1:19">
-      <c r="A341" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B341" s="9">
+        <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 340|Canone 340]] -  -  -  -  -  - </v>
+      </c>
+    </row>
+    <row r="341" spans="1:19" s="1" customFormat="1" ht="13.5" thickBot="1">
+      <c r="A341" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B341" s="3">
         <v>341</v>
       </c>
-      <c r="C341" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D341" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E341" s="9" t="str">
+      <c r="C341" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D341" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E341" s="3" t="str">
         <f t="shared" si="18"/>
         <v>[[Documenti vari/ccar-cic#Canone 341|Canone 341]]</v>
       </c>
-      <c r="F341" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="G341" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="H341" s="9" t="str">
+      <c r="F341" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G341" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H341" s="3" t="str">
         <f t="shared" si="20"/>
         <v>[[Documenti vari/ccar-cic#^ccar-cic-c341-c1|Cm 1]]</v>
       </c>
-      <c r="I341" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="J341" s="9" t="str">
+      <c r="I341" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J341" s="3" t="str">
         <f t="shared" si="21"/>
         <v>[[Documenti vari/ccar-cic#^ccar-cic-c341-c2|Cm 2]]</v>
       </c>
-      <c r="S341" s="9" t="str">
+      <c r="K341" s="3"/>
+      <c r="L341" s="3"/>
+      <c r="M341" s="3"/>
+      <c r="N341" s="3"/>
+      <c r="O341" s="3"/>
+      <c r="P341" s="3"/>
+      <c r="Q341" s="3"/>
+      <c r="R341" s="3"/>
+      <c r="S341" s="3" t="str">
         <f t="shared" si="19"/>
         <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 341|Canone 341]] - [[Documenti vari/ccar-cic#^ccar-cic-c341-c1|Cm 1]] - [[Documenti vari/ccar-cic#^ccar-cic-c341-c2|Cm 2]] -  -  -  - </v>
       </c>
     </row>
-    <row r="342" spans="1:19">
-      <c r="A342" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B342" s="9">
+    <row r="342" spans="1:19" s="1" customFormat="1" ht="13.5" thickTop="1">
+      <c r="A342" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B342" s="1">
         <v>342</v>
       </c>
-      <c r="C342" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D342" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E342" s="9" t="str">
+      <c r="C342" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D342" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E342" s="1" t="str">
         <f t="shared" si="18"/>
         <v>[[Documenti vari/ccar-cic#Canone 342|Canone 342]]</v>
       </c>
-      <c r="F342" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="G342" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="H342" s="9" t="str">
-        <f t="shared" si="20"/>
-        <v>[[Documenti vari/ccar-cic#^ccar-cic-c342-c1|Cm 1]]</v>
-      </c>
-      <c r="I342" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="J342" s="9" t="str">
-        <f t="shared" si="21"/>
-        <v>[[Documenti vari/ccar-cic#^ccar-cic-c342-c2|Cm 2]]</v>
-      </c>
-      <c r="S342" s="9" t="str">
+      <c r="G342" s="2"/>
+      <c r="I342" s="2"/>
+      <c r="S342" s="1" t="str">
         <f t="shared" si="19"/>
-        <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 342|Canone 342]] - [[Documenti vari/ccar-cic#^ccar-cic-c342-c1|Cm 1]] - [[Documenti vari/ccar-cic#^ccar-cic-c342-c2|Cm 2]] -  -  -  - </v>
-      </c>
-    </row>
-    <row r="343" spans="1:19">
-      <c r="A343" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B343" s="9">
+        <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 342|Canone 342]] -  -  -  -  -  - </v>
+      </c>
+    </row>
+    <row r="343" spans="1:19" s="1" customFormat="1">
+      <c r="A343" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B343" s="1">
         <v>343</v>
       </c>
-      <c r="C343" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D343" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E343" s="9" t="str">
+      <c r="C343" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D343" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E343" s="1" t="str">
         <f t="shared" si="18"/>
         <v>[[Documenti vari/ccar-cic#Canone 343|Canone 343]]</v>
       </c>
-      <c r="F343" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="G343" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="H343" s="9" t="str">
-        <f t="shared" si="20"/>
-        <v>[[Documenti vari/ccar-cic#^ccar-cic-c343-c1|Cm 1]]</v>
-      </c>
-      <c r="I343" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="J343" s="9" t="str">
-        <f t="shared" si="21"/>
-        <v>[[Documenti vari/ccar-cic#^ccar-cic-c343-c2|Cm 2]]</v>
-      </c>
-      <c r="S343" s="9" t="str">
+      <c r="G343" s="2"/>
+      <c r="I343" s="2"/>
+      <c r="S343" s="1" t="str">
         <f t="shared" si="19"/>
-        <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 343|Canone 343]] - [[Documenti vari/ccar-cic#^ccar-cic-c343-c1|Cm 1]] - [[Documenti vari/ccar-cic#^ccar-cic-c343-c2|Cm 2]] -  -  -  - </v>
-      </c>
-    </row>
-    <row r="344" spans="1:19">
-      <c r="A344" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B344" s="9">
+        <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 343|Canone 343]] -  -  -  -  -  - </v>
+      </c>
+    </row>
+    <row r="344" spans="1:19" s="1" customFormat="1">
+      <c r="A344" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B344" s="1">
         <v>344</v>
       </c>
-      <c r="C344" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D344" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E344" s="9" t="str">
+      <c r="C344" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D344" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E344" s="1" t="str">
         <f t="shared" si="18"/>
         <v>[[Documenti vari/ccar-cic#Canone 344|Canone 344]]</v>
       </c>
-      <c r="F344" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="G344" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="H344" s="9" t="str">
-        <f t="shared" si="20"/>
-        <v>[[Documenti vari/ccar-cic#^ccar-cic-c344-c1|Cm 1]]</v>
-      </c>
-      <c r="I344" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="J344" s="9" t="str">
-        <f t="shared" si="21"/>
-        <v>[[Documenti vari/ccar-cic#^ccar-cic-c344-c2|Cm 2]]</v>
-      </c>
-      <c r="S344" s="9" t="str">
+      <c r="G344" s="2"/>
+      <c r="I344" s="2"/>
+      <c r="S344" s="1" t="str">
         <f t="shared" si="19"/>
-        <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 344|Canone 344]] - [[Documenti vari/ccar-cic#^ccar-cic-c344-c1|Cm 1]] - [[Documenti vari/ccar-cic#^ccar-cic-c344-c2|Cm 2]] -  -  -  - </v>
-      </c>
-    </row>
-    <row r="345" spans="1:19">
-      <c r="A345" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B345" s="9">
+        <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 344|Canone 344]] -  -  -  -  -  - </v>
+      </c>
+    </row>
+    <row r="345" spans="1:19" s="1" customFormat="1">
+      <c r="A345" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B345" s="1">
         <v>345</v>
       </c>
-      <c r="C345" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D345" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E345" s="9" t="str">
+      <c r="C345" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D345" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E345" s="1" t="str">
         <f t="shared" si="18"/>
         <v>[[Documenti vari/ccar-cic#Canone 345|Canone 345]]</v>
       </c>
-      <c r="F345" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="G345" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="H345" s="9" t="str">
-        <f t="shared" si="20"/>
-        <v>[[Documenti vari/ccar-cic#^ccar-cic-c345-c1|Cm 1]]</v>
-      </c>
-      <c r="I345" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="J345" s="9" t="str">
-        <f t="shared" si="21"/>
-        <v>[[Documenti vari/ccar-cic#^ccar-cic-c345-c2|Cm 2]]</v>
-      </c>
-      <c r="S345" s="9" t="str">
+      <c r="G345" s="2"/>
+      <c r="I345" s="2"/>
+      <c r="S345" s="1" t="str">
         <f t="shared" si="19"/>
-        <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 345|Canone 345]] - [[Documenti vari/ccar-cic#^ccar-cic-c345-c1|Cm 1]] - [[Documenti vari/ccar-cic#^ccar-cic-c345-c2|Cm 2]] -  -  -  - </v>
-      </c>
-    </row>
-    <row r="346" spans="1:19">
-      <c r="A346" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B346" s="9">
+        <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 345|Canone 345]] -  -  -  -  -  - </v>
+      </c>
+    </row>
+    <row r="346" spans="1:19" s="1" customFormat="1">
+      <c r="A346" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B346" s="1">
         <v>346</v>
       </c>
-      <c r="C346" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D346" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E346" s="9" t="str">
+      <c r="C346" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D346" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E346" s="1" t="str">
         <f t="shared" si="18"/>
         <v>[[Documenti vari/ccar-cic#Canone 346|Canone 346]]</v>
       </c>
-      <c r="F346" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="G346" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="H346" s="9" t="str">
+      <c r="F346" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G346" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H346" s="1" t="str">
         <f t="shared" si="20"/>
         <v>[[Documenti vari/ccar-cic#^ccar-cic-c346-c1|Cm 1]]</v>
       </c>
-      <c r="I346" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="J346" s="9" t="str">
+      <c r="I346" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J346" s="1" t="str">
         <f t="shared" si="21"/>
         <v>[[Documenti vari/ccar-cic#^ccar-cic-c346-c2|Cm 2]]</v>
       </c>
-      <c r="S346" s="9" t="str">
+      <c r="K346" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L346" s="1" t="str">
+        <f>_xlfn.CONCAT(F346,B346,K346)</f>
+        <v>[[Documenti vari/ccar-cic#^ccar-cic-c346-c3|Cm 3]]</v>
+      </c>
+      <c r="S346" s="1" t="str">
         <f t="shared" si="19"/>
-        <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 346|Canone 346]] - [[Documenti vari/ccar-cic#^ccar-cic-c346-c1|Cm 1]] - [[Documenti vari/ccar-cic#^ccar-cic-c346-c2|Cm 2]] -  -  -  - </v>
-      </c>
-    </row>
-    <row r="347" spans="1:19">
-      <c r="A347" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B347" s="9">
+        <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 346|Canone 346]] - [[Documenti vari/ccar-cic#^ccar-cic-c346-c1|Cm 1]] - [[Documenti vari/ccar-cic#^ccar-cic-c346-c2|Cm 2]] - [[Documenti vari/ccar-cic#^ccar-cic-c346-c3|Cm 3]] -  -  - </v>
+      </c>
+    </row>
+    <row r="347" spans="1:19" s="1" customFormat="1">
+      <c r="A347" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B347" s="1">
         <v>347</v>
       </c>
-      <c r="C347" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D347" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E347" s="9" t="str">
+      <c r="C347" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D347" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E347" s="1" t="str">
         <f t="shared" si="18"/>
         <v>[[Documenti vari/ccar-cic#Canone 347|Canone 347]]</v>
       </c>
-      <c r="F347" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="G347" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="H347" s="9" t="str">
+      <c r="F347" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G347" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H347" s="1" t="str">
         <f t="shared" si="20"/>
         <v>[[Documenti vari/ccar-cic#^ccar-cic-c347-c1|Cm 1]]</v>
       </c>
-      <c r="I347" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="J347" s="9" t="str">
+      <c r="I347" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J347" s="1" t="str">
         <f t="shared" si="21"/>
         <v>[[Documenti vari/ccar-cic#^ccar-cic-c347-c2|Cm 2]]</v>
       </c>
-      <c r="S347" s="9" t="str">
+      <c r="S347" s="1" t="str">
         <f t="shared" si="19"/>
         <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 347|Canone 347]] - [[Documenti vari/ccar-cic#^ccar-cic-c347-c1|Cm 1]] - [[Documenti vari/ccar-cic#^ccar-cic-c347-c2|Cm 2]] -  -  -  - </v>
       </c>
     </row>
-    <row r="348" spans="1:19">
-      <c r="A348" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B348" s="9">
+    <row r="348" spans="1:19" s="1" customFormat="1" ht="13.5" thickBot="1">
+      <c r="A348" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B348" s="3">
         <v>348</v>
       </c>
-      <c r="C348" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D348" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E348" s="9" t="str">
+      <c r="C348" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D348" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E348" s="3" t="str">
         <f t="shared" si="18"/>
         <v>[[Documenti vari/ccar-cic#Canone 348|Canone 348]]</v>
       </c>
-      <c r="F348" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="G348" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="H348" s="9" t="str">
+      <c r="F348" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G348" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H348" s="3" t="str">
         <f t="shared" si="20"/>
         <v>[[Documenti vari/ccar-cic#^ccar-cic-c348-c1|Cm 1]]</v>
       </c>
-      <c r="I348" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="J348" s="9" t="str">
+      <c r="I348" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J348" s="3" t="str">
         <f t="shared" si="21"/>
         <v>[[Documenti vari/ccar-cic#^ccar-cic-c348-c2|Cm 2]]</v>
       </c>
-      <c r="S348" s="9" t="str">
+      <c r="K348" s="3"/>
+      <c r="L348" s="3"/>
+      <c r="M348" s="3"/>
+      <c r="N348" s="3"/>
+      <c r="O348" s="3"/>
+      <c r="P348" s="3"/>
+      <c r="Q348" s="3"/>
+      <c r="R348" s="3"/>
+      <c r="S348" s="3" t="str">
         <f t="shared" si="19"/>
         <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 348|Canone 348]] - [[Documenti vari/ccar-cic#^ccar-cic-c348-c1|Cm 1]] - [[Documenti vari/ccar-cic#^ccar-cic-c348-c2|Cm 2]] -  -  -  - </v>
       </c>
     </row>
-    <row r="349" spans="1:19">
-      <c r="A349" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B349" s="9">
+    <row r="349" spans="1:19" s="1" customFormat="1" ht="13.5" thickTop="1">
+      <c r="A349" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B349" s="1">
         <v>349</v>
       </c>
-      <c r="C349" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D349" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E349" s="9" t="str">
+      <c r="C349" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D349" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E349" s="1" t="str">
         <f t="shared" si="18"/>
         <v>[[Documenti vari/ccar-cic#Canone 349|Canone 349]]</v>
       </c>
-      <c r="F349" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="G349" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="H349" s="9" t="str">
-        <f t="shared" si="20"/>
-        <v>[[Documenti vari/ccar-cic#^ccar-cic-c349-c1|Cm 1]]</v>
-      </c>
-      <c r="I349" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="J349" s="9" t="str">
-        <f t="shared" si="21"/>
-        <v>[[Documenti vari/ccar-cic#^ccar-cic-c349-c2|Cm 2]]</v>
-      </c>
-      <c r="S349" s="9" t="str">
+      <c r="G349" s="2"/>
+      <c r="I349" s="2"/>
+      <c r="S349" s="1" t="str">
         <f t="shared" si="19"/>
-        <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 349|Canone 349]] - [[Documenti vari/ccar-cic#^ccar-cic-c349-c1|Cm 1]] - [[Documenti vari/ccar-cic#^ccar-cic-c349-c2|Cm 2]] -  -  -  - </v>
-      </c>
-    </row>
-    <row r="350" spans="1:19">
-      <c r="A350" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B350" s="9">
+        <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 349|Canone 349]] -  -  -  -  -  - </v>
+      </c>
+    </row>
+    <row r="350" spans="1:19" s="1" customFormat="1">
+      <c r="A350" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B350" s="1">
         <v>350</v>
       </c>
-      <c r="C350" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D350" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E350" s="9" t="str">
+      <c r="C350" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D350" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E350" s="1" t="str">
         <f t="shared" si="18"/>
         <v>[[Documenti vari/ccar-cic#Canone 350|Canone 350]]</v>
       </c>
-      <c r="F350" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="G350" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="H350" s="9" t="str">
+      <c r="F350" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G350" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H350" s="1" t="str">
         <f t="shared" si="20"/>
         <v>[[Documenti vari/ccar-cic#^ccar-cic-c350-c1|Cm 1]]</v>
       </c>
-      <c r="I350" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="J350" s="9" t="str">
+      <c r="I350" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J350" s="1" t="str">
         <f t="shared" si="21"/>
         <v>[[Documenti vari/ccar-cic#^ccar-cic-c350-c2|Cm 2]]</v>
       </c>
-      <c r="S350" s="9" t="str">
+      <c r="K350" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L350" s="1" t="str">
+        <f>_xlfn.CONCAT(F350,B350,K350)</f>
+        <v>[[Documenti vari/ccar-cic#^ccar-cic-c350-c3|Cm 3]]</v>
+      </c>
+      <c r="M350" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N350" s="1" t="str">
+        <f>_xlfn.CONCAT(F350,B350,M350)</f>
+        <v>[[Documenti vari/ccar-cic#^ccar-cic-c350-c4|Cm 4]]</v>
+      </c>
+      <c r="O350" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="P350" s="1" t="str">
+        <f>_xlfn.CONCAT(F350,B350,O350)</f>
+        <v>[[Documenti vari/ccar-cic#^ccar-cic-c350-c5|Cm 5]]</v>
+      </c>
+      <c r="Q350" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R350" s="1" t="str">
+        <f>_xlfn.CONCAT(F350,B350,Q350)</f>
+        <v>[[Documenti vari/ccar-cic#^ccar-cic-c350-c6|Cm 6]]</v>
+      </c>
+      <c r="S350" s="1" t="str">
         <f t="shared" si="19"/>
-        <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 350|Canone 350]] - [[Documenti vari/ccar-cic#^ccar-cic-c350-c1|Cm 1]] - [[Documenti vari/ccar-cic#^ccar-cic-c350-c2|Cm 2]] -  -  -  - </v>
-      </c>
-    </row>
-    <row r="351" spans="1:19">
-      <c r="A351" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B351" s="9">
+        <v>[[Documenti vari/ccar-cic#Canone 350|Canone 350]] - [[Documenti vari/ccar-cic#^ccar-cic-c350-c1|Cm 1]] - [[Documenti vari/ccar-cic#^ccar-cic-c350-c2|Cm 2]] - [[Documenti vari/ccar-cic#^ccar-cic-c350-c3|Cm 3]] - [[Documenti vari/ccar-cic#^ccar-cic-c350-c4|Cm 4]] - [[Documenti vari/ccar-cic#^ccar-cic-c350-c5|Cm 5]] - [[Documenti vari/ccar-cic#^ccar-cic-c350-c6|Cm 6]]</v>
+      </c>
+    </row>
+    <row r="351" spans="1:19" s="1" customFormat="1">
+      <c r="A351" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B351" s="1">
         <v>351</v>
       </c>
-      <c r="C351" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D351" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E351" s="9" t="str">
+      <c r="C351" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D351" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E351" s="1" t="str">
         <f t="shared" si="18"/>
         <v>[[Documenti vari/ccar-cic#Canone 351|Canone 351]]</v>
       </c>
-      <c r="F351" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="G351" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="H351" s="9" t="str">
+      <c r="F351" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G351" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H351" s="1" t="str">
         <f t="shared" si="20"/>
         <v>[[Documenti vari/ccar-cic#^ccar-cic-c351-c1|Cm 1]]</v>
       </c>
-      <c r="I351" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="J351" s="9" t="str">
+      <c r="I351" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J351" s="1" t="str">
         <f t="shared" si="21"/>
         <v>[[Documenti vari/ccar-cic#^ccar-cic-c351-c2|Cm 2]]</v>
       </c>
-      <c r="S351" s="9" t="str">
+      <c r="K351" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L351" s="1" t="str">
+        <f>_xlfn.CONCAT(F351,B351,K351)</f>
+        <v>[[Documenti vari/ccar-cic#^ccar-cic-c351-c3|Cm 3]]</v>
+      </c>
+      <c r="S351" s="1" t="str">
         <f t="shared" si="19"/>
-        <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 351|Canone 351]] - [[Documenti vari/ccar-cic#^ccar-cic-c351-c1|Cm 1]] - [[Documenti vari/ccar-cic#^ccar-cic-c351-c2|Cm 2]] -  -  -  - </v>
-      </c>
-    </row>
-    <row r="352" spans="1:19">
-      <c r="A352" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B352" s="9">
+        <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 351|Canone 351]] - [[Documenti vari/ccar-cic#^ccar-cic-c351-c1|Cm 1]] - [[Documenti vari/ccar-cic#^ccar-cic-c351-c2|Cm 2]] - [[Documenti vari/ccar-cic#^ccar-cic-c351-c3|Cm 3]] -  -  - </v>
+      </c>
+    </row>
+    <row r="352" spans="1:19" s="1" customFormat="1">
+      <c r="A352" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B352" s="1">
         <v>352</v>
       </c>
-      <c r="C352" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D352" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E352" s="9" t="str">
+      <c r="C352" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D352" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E352" s="1" t="str">
         <f t="shared" si="18"/>
         <v>[[Documenti vari/ccar-cic#Canone 352|Canone 352]]</v>
       </c>
-      <c r="F352" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="G352" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="H352" s="9" t="str">
+      <c r="F352" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G352" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H352" s="1" t="str">
         <f t="shared" si="20"/>
         <v>[[Documenti vari/ccar-cic#^ccar-cic-c352-c1|Cm 1]]</v>
       </c>
-      <c r="I352" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="J352" s="9" t="str">
+      <c r="I352" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J352" s="1" t="str">
         <f t="shared" si="21"/>
         <v>[[Documenti vari/ccar-cic#^ccar-cic-c352-c2|Cm 2]]</v>
       </c>
-      <c r="S352" s="9" t="str">
+      <c r="K352" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L352" s="1" t="str">
+        <f>_xlfn.CONCAT(F352,B352,K352)</f>
+        <v>[[Documenti vari/ccar-cic#^ccar-cic-c352-c3|Cm 3]]</v>
+      </c>
+      <c r="M352" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N352" s="1" t="str">
+        <f>_xlfn.CONCAT(F352,B352,M352)</f>
+        <v>[[Documenti vari/ccar-cic#^ccar-cic-c352-c4|Cm 4]]</v>
+      </c>
+      <c r="S352" s="1" t="str">
         <f t="shared" si="19"/>
-        <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 352|Canone 352]] - [[Documenti vari/ccar-cic#^ccar-cic-c352-c1|Cm 1]] - [[Documenti vari/ccar-cic#^ccar-cic-c352-c2|Cm 2]] -  -  -  - </v>
-      </c>
-    </row>
-    <row r="353" spans="1:19">
-      <c r="A353" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B353" s="9">
+        <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 352|Canone 352]] - [[Documenti vari/ccar-cic#^ccar-cic-c352-c1|Cm 1]] - [[Documenti vari/ccar-cic#^ccar-cic-c352-c2|Cm 2]] - [[Documenti vari/ccar-cic#^ccar-cic-c352-c3|Cm 3]] - [[Documenti vari/ccar-cic#^ccar-cic-c352-c4|Cm 4]] -  - </v>
+      </c>
+    </row>
+    <row r="353" spans="1:19" s="1" customFormat="1">
+      <c r="A353" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B353" s="1">
         <v>353</v>
       </c>
-      <c r="C353" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D353" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E353" s="9" t="str">
+      <c r="C353" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D353" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E353" s="1" t="str">
         <f t="shared" si="18"/>
         <v>[[Documenti vari/ccar-cic#Canone 353|Canone 353]]</v>
       </c>
-      <c r="F353" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="G353" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="H353" s="9" t="str">
+      <c r="F353" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G353" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H353" s="1" t="str">
         <f t="shared" si="20"/>
         <v>[[Documenti vari/ccar-cic#^ccar-cic-c353-c1|Cm 1]]</v>
       </c>
-      <c r="I353" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="J353" s="9" t="str">
+      <c r="I353" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J353" s="1" t="str">
         <f t="shared" si="21"/>
         <v>[[Documenti vari/ccar-cic#^ccar-cic-c353-c2|Cm 2]]</v>
       </c>
-      <c r="S353" s="9" t="str">
+      <c r="K353" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L353" s="1" t="str">
+        <f>_xlfn.CONCAT(F353,B353,K353)</f>
+        <v>[[Documenti vari/ccar-cic#^ccar-cic-c353-c3|Cm 3]]</v>
+      </c>
+      <c r="M353" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N353" s="1" t="str">
+        <f>_xlfn.CONCAT(F353,B353,M353)</f>
+        <v>[[Documenti vari/ccar-cic#^ccar-cic-c353-c4|Cm 4]]</v>
+      </c>
+      <c r="S353" s="1" t="str">
         <f t="shared" si="19"/>
-        <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 353|Canone 353]] - [[Documenti vari/ccar-cic#^ccar-cic-c353-c1|Cm 1]] - [[Documenti vari/ccar-cic#^ccar-cic-c353-c2|Cm 2]] -  -  -  - </v>
-      </c>
-    </row>
-    <row r="354" spans="1:19">
-      <c r="A354" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B354" s="9">
+        <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 353|Canone 353]] - [[Documenti vari/ccar-cic#^ccar-cic-c353-c1|Cm 1]] - [[Documenti vari/ccar-cic#^ccar-cic-c353-c2|Cm 2]] - [[Documenti vari/ccar-cic#^ccar-cic-c353-c3|Cm 3]] - [[Documenti vari/ccar-cic#^ccar-cic-c353-c4|Cm 4]] -  - </v>
+      </c>
+    </row>
+    <row r="354" spans="1:19" s="1" customFormat="1">
+      <c r="A354" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B354" s="1">
         <v>354</v>
       </c>
-      <c r="C354" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D354" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E354" s="9" t="str">
+      <c r="C354" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D354" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E354" s="1" t="str">
         <f t="shared" si="18"/>
         <v>[[Documenti vari/ccar-cic#Canone 354|Canone 354]]</v>
       </c>
-      <c r="F354" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="G354" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="H354" s="9" t="str">
-        <f t="shared" si="20"/>
-        <v>[[Documenti vari/ccar-cic#^ccar-cic-c354-c1|Cm 1]]</v>
-      </c>
-      <c r="I354" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="J354" s="9" t="str">
-        <f t="shared" si="21"/>
-        <v>[[Documenti vari/ccar-cic#^ccar-cic-c354-c2|Cm 2]]</v>
-      </c>
-      <c r="S354" s="9" t="str">
+      <c r="G354" s="2"/>
+      <c r="I354" s="2"/>
+      <c r="S354" s="1" t="str">
         <f t="shared" si="19"/>
-        <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 354|Canone 354]] - [[Documenti vari/ccar-cic#^ccar-cic-c354-c1|Cm 1]] - [[Documenti vari/ccar-cic#^ccar-cic-c354-c2|Cm 2]] -  -  -  - </v>
-      </c>
-    </row>
-    <row r="355" spans="1:19">
-      <c r="A355" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B355" s="9">
+        <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 354|Canone 354]] -  -  -  -  -  - </v>
+      </c>
+    </row>
+    <row r="355" spans="1:19" s="1" customFormat="1">
+      <c r="A355" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B355" s="1">
         <v>355</v>
       </c>
-      <c r="C355" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D355" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E355" s="9" t="str">
+      <c r="C355" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D355" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E355" s="1" t="str">
         <f t="shared" si="18"/>
         <v>[[Documenti vari/ccar-cic#Canone 355|Canone 355]]</v>
       </c>
-      <c r="F355" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="G355" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="H355" s="9" t="str">
+      <c r="F355" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G355" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H355" s="1" t="str">
         <f t="shared" si="20"/>
         <v>[[Documenti vari/ccar-cic#^ccar-cic-c355-c1|Cm 1]]</v>
       </c>
-      <c r="I355" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="J355" s="9" t="str">
+      <c r="I355" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J355" s="1" t="str">
         <f t="shared" si="21"/>
         <v>[[Documenti vari/ccar-cic#^ccar-cic-c355-c2|Cm 2]]</v>
       </c>
-      <c r="S355" s="9" t="str">
+      <c r="S355" s="1" t="str">
         <f t="shared" si="19"/>
         <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 355|Canone 355]] - [[Documenti vari/ccar-cic#^ccar-cic-c355-c1|Cm 1]] - [[Documenti vari/ccar-cic#^ccar-cic-c355-c2|Cm 2]] -  -  -  - </v>
       </c>
     </row>
-    <row r="356" spans="1:19">
-      <c r="A356" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B356" s="9">
+    <row r="356" spans="1:19" s="1" customFormat="1">
+      <c r="A356" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B356" s="1">
         <v>356</v>
       </c>
-      <c r="C356" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D356" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E356" s="9" t="str">
+      <c r="C356" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D356" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E356" s="1" t="str">
         <f t="shared" si="18"/>
         <v>[[Documenti vari/ccar-cic#Canone 356|Canone 356]]</v>
       </c>
-      <c r="F356" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="G356" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="H356" s="9" t="str">
-        <f t="shared" si="20"/>
-        <v>[[Documenti vari/ccar-cic#^ccar-cic-c356-c1|Cm 1]]</v>
-      </c>
-      <c r="I356" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="J356" s="9" t="str">
-        <f t="shared" si="21"/>
-        <v>[[Documenti vari/ccar-cic#^ccar-cic-c356-c2|Cm 2]]</v>
-      </c>
-      <c r="S356" s="9" t="str">
+      <c r="G356" s="2"/>
+      <c r="I356" s="2"/>
+      <c r="S356" s="1" t="str">
         <f t="shared" si="19"/>
-        <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 356|Canone 356]] - [[Documenti vari/ccar-cic#^ccar-cic-c356-c1|Cm 1]] - [[Documenti vari/ccar-cic#^ccar-cic-c356-c2|Cm 2]] -  -  -  - </v>
-      </c>
-    </row>
-    <row r="357" spans="1:19">
-      <c r="A357" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B357" s="9">
+        <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 356|Canone 356]] -  -  -  -  -  - </v>
+      </c>
+    </row>
+    <row r="357" spans="1:19" s="1" customFormat="1">
+      <c r="A357" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B357" s="1">
         <v>357</v>
       </c>
-      <c r="C357" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D357" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E357" s="9" t="str">
+      <c r="C357" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D357" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E357" s="1" t="str">
         <f t="shared" si="18"/>
         <v>[[Documenti vari/ccar-cic#Canone 357|Canone 357]]</v>
       </c>
-      <c r="F357" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="G357" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="H357" s="9" t="str">
+      <c r="F357" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G357" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H357" s="1" t="str">
         <f t="shared" si="20"/>
         <v>[[Documenti vari/ccar-cic#^ccar-cic-c357-c1|Cm 1]]</v>
       </c>
-      <c r="I357" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="J357" s="9" t="str">
+      <c r="I357" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J357" s="1" t="str">
         <f t="shared" si="21"/>
         <v>[[Documenti vari/ccar-cic#^ccar-cic-c357-c2|Cm 2]]</v>
       </c>
-      <c r="S357" s="9" t="str">
+      <c r="S357" s="1" t="str">
         <f t="shared" si="19"/>
         <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 357|Canone 357]] - [[Documenti vari/ccar-cic#^ccar-cic-c357-c1|Cm 1]] - [[Documenti vari/ccar-cic#^ccar-cic-c357-c2|Cm 2]] -  -  -  - </v>
       </c>
     </row>
-    <row r="358" spans="1:19">
-      <c r="A358" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B358" s="9">
+    <row r="358" spans="1:19" s="1" customFormat="1">
+      <c r="A358" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B358" s="1">
         <v>358</v>
       </c>
-      <c r="C358" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D358" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E358" s="9" t="str">
+      <c r="C358" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D358" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E358" s="1" t="str">
         <f t="shared" si="18"/>
         <v>[[Documenti vari/ccar-cic#Canone 358|Canone 358]]</v>
       </c>
-      <c r="F358" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="G358" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="H358" s="9" t="str">
-        <f t="shared" si="20"/>
-        <v>[[Documenti vari/ccar-cic#^ccar-cic-c358-c1|Cm 1]]</v>
-      </c>
-      <c r="I358" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="J358" s="9" t="str">
-        <f t="shared" si="21"/>
-        <v>[[Documenti vari/ccar-cic#^ccar-cic-c358-c2|Cm 2]]</v>
-      </c>
-      <c r="S358" s="9" t="str">
+      <c r="G358" s="2"/>
+      <c r="I358" s="2"/>
+      <c r="S358" s="1" t="str">
         <f t="shared" si="19"/>
-        <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 358|Canone 358]] - [[Documenti vari/ccar-cic#^ccar-cic-c358-c1|Cm 1]] - [[Documenti vari/ccar-cic#^ccar-cic-c358-c2|Cm 2]] -  -  -  - </v>
-      </c>
-    </row>
-    <row r="359" spans="1:19">
-      <c r="A359" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B359" s="9">
+        <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 358|Canone 358]] -  -  -  -  -  - </v>
+      </c>
+    </row>
+    <row r="359" spans="1:19" s="1" customFormat="1" ht="13.5" thickBot="1">
+      <c r="A359" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B359" s="3">
         <v>359</v>
       </c>
-      <c r="C359" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D359" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E359" s="9" t="str">
+      <c r="C359" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D359" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E359" s="3" t="str">
         <f t="shared" si="18"/>
         <v>[[Documenti vari/ccar-cic#Canone 359|Canone 359]]</v>
       </c>
-      <c r="F359" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="G359" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="H359" s="9" t="str">
-        <f t="shared" si="20"/>
-        <v>[[Documenti vari/ccar-cic#^ccar-cic-c359-c1|Cm 1]]</v>
-      </c>
-      <c r="I359" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="J359" s="9" t="str">
-        <f t="shared" si="21"/>
-        <v>[[Documenti vari/ccar-cic#^ccar-cic-c359-c2|Cm 2]]</v>
-      </c>
-      <c r="S359" s="9" t="str">
+      <c r="F359" s="3"/>
+      <c r="G359" s="4"/>
+      <c r="H359" s="3"/>
+      <c r="I359" s="4"/>
+      <c r="J359" s="3"/>
+      <c r="K359" s="3"/>
+      <c r="L359" s="3"/>
+      <c r="M359" s="3"/>
+      <c r="N359" s="3"/>
+      <c r="O359" s="3"/>
+      <c r="P359" s="3"/>
+      <c r="Q359" s="3"/>
+      <c r="R359" s="3"/>
+      <c r="S359" s="3" t="str">
         <f t="shared" si="19"/>
-        <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 359|Canone 359]] - [[Documenti vari/ccar-cic#^ccar-cic-c359-c1|Cm 1]] - [[Documenti vari/ccar-cic#^ccar-cic-c359-c2|Cm 2]] -  -  -  - </v>
-      </c>
-    </row>
-    <row r="360" spans="1:19">
-      <c r="A360" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B360" s="9">
+        <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 359|Canone 359]] -  -  -  -  -  - </v>
+      </c>
+    </row>
+    <row r="360" spans="1:19" s="1" customFormat="1" ht="13.5" thickTop="1">
+      <c r="A360" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B360" s="1">
         <v>360</v>
       </c>
-      <c r="C360" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D360" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E360" s="9" t="str">
+      <c r="C360" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D360" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E360" s="1" t="str">
         <f t="shared" si="18"/>
         <v>[[Documenti vari/ccar-cic#Canone 360|Canone 360]]</v>
       </c>
-      <c r="F360" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="G360" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="H360" s="9" t="str">
-        <f t="shared" si="20"/>
-        <v>[[Documenti vari/ccar-cic#^ccar-cic-c360-c1|Cm 1]]</v>
-      </c>
-      <c r="I360" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="J360" s="9" t="str">
-        <f t="shared" si="21"/>
-        <v>[[Documenti vari/ccar-cic#^ccar-cic-c360-c2|Cm 2]]</v>
-      </c>
-      <c r="S360" s="9" t="str">
+      <c r="G360" s="2"/>
+      <c r="I360" s="2"/>
+      <c r="S360" s="1" t="str">
         <f t="shared" si="19"/>
-        <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 360|Canone 360]] - [[Documenti vari/ccar-cic#^ccar-cic-c360-c1|Cm 1]] - [[Documenti vari/ccar-cic#^ccar-cic-c360-c2|Cm 2]] -  -  -  - </v>
-      </c>
-    </row>
-    <row r="361" spans="1:19">
-      <c r="A361" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B361" s="9">
+        <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 360|Canone 360]] -  -  -  -  -  - </v>
+      </c>
+    </row>
+    <row r="361" spans="1:19" s="1" customFormat="1" ht="13.5" thickBot="1">
+      <c r="A361" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B361" s="3">
         <v>361</v>
       </c>
-      <c r="C361" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D361" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E361" s="9" t="str">
+      <c r="C361" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D361" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E361" s="3" t="str">
         <f t="shared" si="18"/>
         <v>[[Documenti vari/ccar-cic#Canone 361|Canone 361]]</v>
       </c>
-      <c r="F361" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="G361" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="H361" s="9" t="str">
-        <f t="shared" si="20"/>
-        <v>[[Documenti vari/ccar-cic#^ccar-cic-c361-c1|Cm 1]]</v>
-      </c>
-      <c r="I361" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="J361" s="9" t="str">
-        <f t="shared" si="21"/>
-        <v>[[Documenti vari/ccar-cic#^ccar-cic-c361-c2|Cm 2]]</v>
-      </c>
-      <c r="S361" s="9" t="str">
+      <c r="F361" s="3"/>
+      <c r="G361" s="4"/>
+      <c r="H361" s="3"/>
+      <c r="I361" s="4"/>
+      <c r="J361" s="3"/>
+      <c r="K361" s="3"/>
+      <c r="L361" s="3"/>
+      <c r="M361" s="3"/>
+      <c r="N361" s="3"/>
+      <c r="O361" s="3"/>
+      <c r="P361" s="3"/>
+      <c r="Q361" s="3"/>
+      <c r="R361" s="3"/>
+      <c r="S361" s="3" t="str">
         <f t="shared" si="19"/>
-        <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 361|Canone 361]] - [[Documenti vari/ccar-cic#^ccar-cic-c361-c1|Cm 1]] - [[Documenti vari/ccar-cic#^ccar-cic-c361-c2|Cm 2]] -  -  -  - </v>
-      </c>
-    </row>
-    <row r="362" spans="1:19">
-      <c r="A362" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B362" s="9">
+        <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 361|Canone 361]] -  -  -  -  -  - </v>
+      </c>
+    </row>
+    <row r="362" spans="1:19" s="1" customFormat="1" ht="13.5" thickTop="1">
+      <c r="A362" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B362" s="1">
         <v>362</v>
       </c>
-      <c r="C362" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D362" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E362" s="9" t="str">
+      <c r="C362" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D362" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E362" s="1" t="str">
         <f t="shared" si="18"/>
         <v>[[Documenti vari/ccar-cic#Canone 362|Canone 362]]</v>
       </c>
-      <c r="F362" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="G362" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="H362" s="9" t="str">
-        <f t="shared" si="20"/>
-        <v>[[Documenti vari/ccar-cic#^ccar-cic-c362-c1|Cm 1]]</v>
-      </c>
-      <c r="I362" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="J362" s="9" t="str">
-        <f t="shared" si="21"/>
-        <v>[[Documenti vari/ccar-cic#^ccar-cic-c362-c2|Cm 2]]</v>
-      </c>
-      <c r="S362" s="9" t="str">
+      <c r="G362" s="2"/>
+      <c r="I362" s="2"/>
+      <c r="S362" s="1" t="str">
         <f t="shared" si="19"/>
-        <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 362|Canone 362]] - [[Documenti vari/ccar-cic#^ccar-cic-c362-c1|Cm 1]] - [[Documenti vari/ccar-cic#^ccar-cic-c362-c2|Cm 2]] -  -  -  - </v>
-      </c>
-    </row>
-    <row r="363" spans="1:19">
-      <c r="A363" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B363" s="9">
+        <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 362|Canone 362]] -  -  -  -  -  - </v>
+      </c>
+    </row>
+    <row r="363" spans="1:19" s="1" customFormat="1">
+      <c r="A363" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B363" s="1">
         <v>363</v>
       </c>
-      <c r="C363" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D363" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E363" s="9" t="str">
+      <c r="C363" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D363" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E363" s="1" t="str">
         <f t="shared" si="18"/>
         <v>[[Documenti vari/ccar-cic#Canone 363|Canone 363]]</v>
       </c>
-      <c r="F363" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="G363" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="H363" s="9" t="str">
+      <c r="F363" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G363" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H363" s="1" t="str">
         <f t="shared" si="20"/>
         <v>[[Documenti vari/ccar-cic#^ccar-cic-c363-c1|Cm 1]]</v>
       </c>
-      <c r="I363" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="J363" s="9" t="str">
+      <c r="I363" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J363" s="1" t="str">
         <f t="shared" si="21"/>
         <v>[[Documenti vari/ccar-cic#^ccar-cic-c363-c2|Cm 2]]</v>
       </c>
-      <c r="S363" s="9" t="str">
+      <c r="S363" s="1" t="str">
         <f t="shared" si="19"/>
         <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 363|Canone 363]] - [[Documenti vari/ccar-cic#^ccar-cic-c363-c1|Cm 1]] - [[Documenti vari/ccar-cic#^ccar-cic-c363-c2|Cm 2]] -  -  -  - </v>
       </c>
     </row>
-    <row r="364" spans="1:19">
-      <c r="A364" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B364" s="9">
+    <row r="364" spans="1:19" s="1" customFormat="1">
+      <c r="A364" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B364" s="1">
         <v>364</v>
       </c>
-      <c r="C364" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D364" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E364" s="9" t="str">
+      <c r="C364" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D364" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E364" s="1" t="str">
         <f t="shared" si="18"/>
         <v>[[Documenti vari/ccar-cic#Canone 364|Canone 364]]</v>
       </c>
-      <c r="F364" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="G364" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="H364" s="9" t="str">
-        <f t="shared" si="20"/>
-        <v>[[Documenti vari/ccar-cic#^ccar-cic-c364-c1|Cm 1]]</v>
-      </c>
-      <c r="I364" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="J364" s="9" t="str">
-        <f t="shared" si="21"/>
-        <v>[[Documenti vari/ccar-cic#^ccar-cic-c364-c2|Cm 2]]</v>
-      </c>
-      <c r="S364" s="9" t="str">
+      <c r="G364" s="2"/>
+      <c r="I364" s="2"/>
+      <c r="S364" s="1" t="str">
         <f t="shared" si="19"/>
-        <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 364|Canone 364]] - [[Documenti vari/ccar-cic#^ccar-cic-c364-c1|Cm 1]] - [[Documenti vari/ccar-cic#^ccar-cic-c364-c2|Cm 2]] -  -  -  - </v>
-      </c>
-    </row>
-    <row r="365" spans="1:19">
-      <c r="A365" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B365" s="9">
+        <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 364|Canone 364]] -  -  -  -  -  - </v>
+      </c>
+    </row>
+    <row r="365" spans="1:19" s="1" customFormat="1">
+      <c r="A365" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B365" s="1">
         <v>365</v>
       </c>
-      <c r="C365" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D365" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E365" s="9" t="str">
+      <c r="C365" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D365" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E365" s="1" t="str">
         <f t="shared" si="18"/>
         <v>[[Documenti vari/ccar-cic#Canone 365|Canone 365]]</v>
       </c>
-      <c r="F365" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="G365" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="H365" s="9" t="str">
+      <c r="F365" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G365" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H365" s="1" t="str">
         <f t="shared" si="20"/>
         <v>[[Documenti vari/ccar-cic#^ccar-cic-c365-c1|Cm 1]]</v>
       </c>
-      <c r="I365" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="J365" s="9" t="str">
+      <c r="I365" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J365" s="1" t="str">
         <f t="shared" si="21"/>
         <v>[[Documenti vari/ccar-cic#^ccar-cic-c365-c2|Cm 2]]</v>
       </c>
-      <c r="S365" s="9" t="str">
+      <c r="S365" s="1" t="str">
         <f t="shared" si="19"/>
         <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 365|Canone 365]] - [[Documenti vari/ccar-cic#^ccar-cic-c365-c1|Cm 1]] - [[Documenti vari/ccar-cic#^ccar-cic-c365-c2|Cm 2]] -  -  -  - </v>
       </c>
     </row>
-    <row r="366" spans="1:19">
-      <c r="A366" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B366" s="9">
+    <row r="366" spans="1:19" s="1" customFormat="1">
+      <c r="A366" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B366" s="1">
         <v>366</v>
       </c>
-      <c r="C366" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D366" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E366" s="9" t="str">
+      <c r="C366" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D366" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E366" s="1" t="str">
         <f t="shared" si="18"/>
         <v>[[Documenti vari/ccar-cic#Canone 366|Canone 366]]</v>
       </c>
-      <c r="F366" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="G366" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="H366" s="9" t="str">
-        <f t="shared" si="20"/>
-        <v>[[Documenti vari/ccar-cic#^ccar-cic-c366-c1|Cm 1]]</v>
-      </c>
-      <c r="I366" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="J366" s="9" t="str">
-        <f t="shared" si="21"/>
-        <v>[[Documenti vari/ccar-cic#^ccar-cic-c366-c2|Cm 2]]</v>
-      </c>
-      <c r="S366" s="9" t="str">
+      <c r="G366" s="2"/>
+      <c r="I366" s="2"/>
+      <c r="S366" s="1" t="str">
         <f t="shared" si="19"/>
-        <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 366|Canone 366]] - [[Documenti vari/ccar-cic#^ccar-cic-c366-c1|Cm 1]] - [[Documenti vari/ccar-cic#^ccar-cic-c366-c2|Cm 2]] -  -  -  - </v>
-      </c>
-    </row>
-    <row r="367" spans="1:19">
-      <c r="A367" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B367" s="9">
+        <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 366|Canone 366]] -  -  -  -  -  - </v>
+      </c>
+    </row>
+    <row r="367" spans="1:19" s="1" customFormat="1" ht="13.5" thickBot="1">
+      <c r="A367" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B367" s="3">
         <v>367</v>
       </c>
-      <c r="C367" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D367" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E367" s="9" t="str">
+      <c r="C367" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D367" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E367" s="3" t="str">
         <f t="shared" si="18"/>
         <v>[[Documenti vari/ccar-cic#Canone 367|Canone 367]]</v>
       </c>
-      <c r="F367" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="G367" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="H367" s="9" t="str">
-        <f t="shared" si="20"/>
-        <v>[[Documenti vari/ccar-cic#^ccar-cic-c367-c1|Cm 1]]</v>
-      </c>
-      <c r="I367" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="J367" s="9" t="str">
-        <f t="shared" si="21"/>
-        <v>[[Documenti vari/ccar-cic#^ccar-cic-c367-c2|Cm 2]]</v>
-      </c>
-      <c r="S367" s="9" t="str">
+      <c r="F367" s="3"/>
+      <c r="G367" s="4"/>
+      <c r="H367" s="3"/>
+      <c r="I367" s="4"/>
+      <c r="J367" s="3"/>
+      <c r="K367" s="3"/>
+      <c r="L367" s="3"/>
+      <c r="M367" s="3"/>
+      <c r="N367" s="3"/>
+      <c r="O367" s="3"/>
+      <c r="P367" s="3"/>
+      <c r="Q367" s="3"/>
+      <c r="R367" s="3"/>
+      <c r="S367" s="3" t="str">
         <f t="shared" si="19"/>
-        <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 367|Canone 367]] - [[Documenti vari/ccar-cic#^ccar-cic-c367-c1|Cm 1]] - [[Documenti vari/ccar-cic#^ccar-cic-c367-c2|Cm 2]] -  -  -  - </v>
-      </c>
-    </row>
-    <row r="368" spans="1:19">
+        <v xml:space="preserve">[[Documenti vari/ccar-cic#Canone 367|Canone 367]] -  -  -  -  -  - </v>
+      </c>
+    </row>
+    <row r="368" spans="1:19" ht="13.5" thickTop="1">
       <c r="A368" s="9" t="s">
         <v>5</v>
       </c>

</xml_diff>